<commit_message>
Capturing state prior to changing how cross validation reported on
</commit_message>
<xml_diff>
--- a/genomes_false_calls_exploration.xlsx
+++ b/genomes_false_calls_exploration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="0" windowWidth="25360" windowHeight="17300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="25360" windowHeight="17300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pcr_plus_false_calls_Exact Pair" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="145">
   <si>
     <t>index1</t>
   </si>
@@ -451,6 +451,12 @@
   <si>
     <t>rest</t>
   </si>
+  <si>
+    <t>23 false diffs</t>
+  </si>
+  <si>
+    <t>out of how many possible?</t>
+  </si>
 </sst>
 </file>
 
@@ -498,8 +504,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -576,7 +586,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -613,6 +623,8 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -649,6 +661,8 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2549,10 +2563,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2615,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(D2=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F2:F33" si="0">IF(D2=0,"false_diff","false_same")</f>
         <v>false_diff</v>
       </c>
       <c r="G2" t="s">
@@ -2657,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(D3=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G3" t="s">
@@ -2699,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(D4=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G4" t="s">
@@ -2741,7 +2755,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(D5=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G5" t="s">
@@ -2783,7 +2797,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(D6=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G6" t="s">
@@ -2825,7 +2839,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(D7=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G7" t="s">
@@ -2867,7 +2881,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="str">
-        <f>IF(D8=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G8" t="s">
@@ -2909,7 +2923,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(D9=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G9" t="s">
@@ -2951,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="str">
-        <f>IF(D10=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G10" t="s">
@@ -2993,7 +3007,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="str">
-        <f>IF(D11=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G11" t="s">
@@ -3035,7 +3049,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="str">
-        <f>IF(D12=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G12" t="s">
@@ -3077,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="str">
-        <f>IF(D13=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G13" t="s">
@@ -3119,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="str">
-        <f>IF(D14=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G14" t="s">
@@ -3161,7 +3175,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="str">
-        <f>IF(D15=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G15" t="s">
@@ -3203,7 +3217,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="str">
-        <f>IF(D16=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G16" t="s">
@@ -3245,7 +3259,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="str">
-        <f>IF(D17=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G17" t="s">
@@ -3287,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="str">
-        <f>IF(D18=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G18" t="s">
@@ -3329,7 +3343,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="str">
-        <f>IF(D19=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G19" t="s">
@@ -3371,7 +3385,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="str">
-        <f>IF(D20=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G20" t="s">
@@ -3413,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="str">
-        <f>IF(D21=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G21" t="s">
@@ -3455,7 +3469,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="str">
-        <f>IF(D22=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G22" t="s">
@@ -3497,7 +3511,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="str">
-        <f>IF(D23=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G23" t="s">
@@ -3539,7 +3553,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="str">
-        <f>IF(D24=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G24" t="s">
@@ -3581,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="str">
-        <f>IF(D25=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G25" t="s">
@@ -3623,7 +3637,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="str">
-        <f>IF(D26=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G26" t="s">
@@ -3665,7 +3679,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="str">
-        <f>IF(D27=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G27" t="s">
@@ -3707,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="str">
-        <f>IF(D28=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G28" t="s">
@@ -3749,7 +3763,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="str">
-        <f>IF(D29=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G29" t="s">
@@ -3791,7 +3805,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="str">
-        <f>IF(D30=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G30" t="s">
@@ -3833,7 +3847,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="str">
-        <f>IF(D31=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G31" t="s">
@@ -3875,7 +3889,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="str">
-        <f>IF(D32=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G32" t="s">
@@ -3917,7 +3931,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="str">
-        <f>IF(D33=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G33" t="s">
@@ -3959,7 +3973,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="str">
-        <f>IF(D34=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F34:F59" si="1">IF(D34=0,"false_diff","false_same")</f>
         <v>false_diff</v>
       </c>
       <c r="G34" t="s">
@@ -4001,7 +4015,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="str">
-        <f>IF(D35=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G35" t="s">
@@ -4043,7 +4057,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="str">
-        <f>IF(D36=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G36" t="s">
@@ -4085,7 +4099,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="str">
-        <f>IF(D37=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G37" t="s">
@@ -4127,7 +4141,7 @@
         <v>1</v>
       </c>
       <c r="F38" t="str">
-        <f>IF(D38=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G38" t="s">
@@ -4169,7 +4183,7 @@
         <v>1</v>
       </c>
       <c r="F39" t="str">
-        <f>IF(D39=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G39" t="s">
@@ -4211,7 +4225,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="str">
-        <f>IF(D40=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G40" t="s">
@@ -4253,7 +4267,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="str">
-        <f>IF(D41=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G41" t="s">
@@ -4295,7 +4309,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="str">
-        <f>IF(D42=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G42" t="s">
@@ -4337,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="str">
-        <f>IF(D43=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G43" t="s">
@@ -4379,7 +4393,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="str">
-        <f>IF(D44=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G44" t="s">
@@ -4421,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="str">
-        <f>IF(D45=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G45" t="s">
@@ -4463,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="str">
-        <f>IF(D46=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G46" t="s">
@@ -4505,7 +4519,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="str">
-        <f>IF(D47=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G47" t="s">
@@ -4547,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="str">
-        <f>IF(D48=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G48" t="s">
@@ -4589,7 +4603,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="str">
-        <f>IF(D49=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G49" t="s">
@@ -4631,7 +4645,7 @@
         <v>0</v>
       </c>
       <c r="F50" t="str">
-        <f>IF(D50=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G50" t="s">
@@ -4673,7 +4687,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="str">
-        <f>IF(D51=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G51" t="s">
@@ -4715,7 +4729,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="str">
-        <f>IF(D52=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G52" t="s">
@@ -4757,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="str">
-        <f>IF(D53=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G53" t="s">
@@ -4799,7 +4813,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="str">
-        <f>IF(D54=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G54" t="s">
@@ -4841,7 +4855,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="str">
-        <f>IF(D55=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G55" t="s">
@@ -4883,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="str">
-        <f>IF(D56=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G56" t="s">
@@ -4925,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="str">
-        <f>IF(D57=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G57" t="s">
@@ -4967,7 +4981,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="str">
-        <f>IF(D58=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G58" t="s">
@@ -5009,7 +5023,7 @@
         <v>0</v>
       </c>
       <c r="F59" t="str">
-        <f>IF(D59=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_same</v>
       </c>
       <c r="G59" t="s">
@@ -5073,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <f t="shared" ref="J63:J64" si="0">SUM(H63:I63)</f>
+        <f t="shared" ref="J63:J64" si="2">SUM(H63:I63)</f>
         <v>23</v>
       </c>
     </row>
@@ -5089,7 +5103,7 @@
         <v>12</v>
       </c>
       <c r="J64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
@@ -5108,6 +5122,21 @@
       <c r="J65">
         <f>COUNTA(F2:F59)</f>
         <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="7:10">
+      <c r="H69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="7:10">
+      <c r="H70" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="7:10">
+      <c r="H72">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5217,7 +5246,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(D2=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F2:F65" si="0">IF(D2=0,"false_diff","false_same")</f>
         <v>false_diff</v>
       </c>
       <c r="G2" t="s">
@@ -5259,7 +5288,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(D3=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G3" t="s">
@@ -5301,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(D4=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G4" t="s">
@@ -5343,7 +5372,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(D5=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G5" t="s">
@@ -5385,7 +5414,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(D6=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G6" t="s">
@@ -5427,7 +5456,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(D7=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G7" t="s">
@@ -5469,7 +5498,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="str">
-        <f>IF(D8=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G8" t="s">
@@ -5511,7 +5540,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(D9=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G9" t="s">
@@ -5553,7 +5582,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="str">
-        <f>IF(D10=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G10" t="s">
@@ -5595,7 +5624,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="str">
-        <f>IF(D11=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G11" t="s">
@@ -5637,7 +5666,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="str">
-        <f>IF(D12=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G12" t="s">
@@ -5679,7 +5708,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="str">
-        <f>IF(D13=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G13" t="s">
@@ -5721,7 +5750,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="str">
-        <f>IF(D14=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G14" t="s">
@@ -5763,7 +5792,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="str">
-        <f>IF(D15=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G15" t="s">
@@ -5805,7 +5834,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="str">
-        <f>IF(D16=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G16" t="s">
@@ -5847,7 +5876,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="str">
-        <f>IF(D17=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G17" t="s">
@@ -5889,7 +5918,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="str">
-        <f>IF(D18=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G18" t="s">
@@ -5931,7 +5960,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="str">
-        <f>IF(D19=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G19" t="s">
@@ -5973,7 +6002,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="str">
-        <f>IF(D20=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G20" t="s">
@@ -6015,7 +6044,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="str">
-        <f>IF(D21=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G21" t="s">
@@ -6057,7 +6086,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="str">
-        <f>IF(D22=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G22" t="s">
@@ -6099,7 +6128,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="str">
-        <f>IF(D23=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G23" t="s">
@@ -6141,7 +6170,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="str">
-        <f>IF(D24=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G24" t="s">
@@ -6183,7 +6212,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="str">
-        <f>IF(D25=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G25" t="s">
@@ -6225,7 +6254,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="str">
-        <f>IF(D26=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G26" t="s">
@@ -6267,7 +6296,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="str">
-        <f>IF(D27=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G27" t="s">
@@ -6309,7 +6338,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="str">
-        <f>IF(D28=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G28" t="s">
@@ -6351,7 +6380,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="str">
-        <f>IF(D29=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G29" t="s">
@@ -6393,7 +6422,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="str">
-        <f>IF(D30=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G30" t="s">
@@ -6435,7 +6464,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="str">
-        <f>IF(D31=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G31" t="s">
@@ -6477,7 +6506,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="str">
-        <f>IF(D32=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G32" t="s">
@@ -6519,7 +6548,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="str">
-        <f>IF(D33=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G33" t="s">
@@ -6561,7 +6590,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="str">
-        <f>IF(D34=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G34" t="s">
@@ -6603,7 +6632,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="str">
-        <f>IF(D35=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G35" t="s">
@@ -6645,7 +6674,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="str">
-        <f>IF(D36=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G36" t="s">
@@ -6687,7 +6716,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="str">
-        <f>IF(D37=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G37" t="s">
@@ -6729,7 +6758,7 @@
         <v>1</v>
       </c>
       <c r="F38" t="str">
-        <f>IF(D38=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G38" t="s">
@@ -6771,7 +6800,7 @@
         <v>1</v>
       </c>
       <c r="F39" t="str">
-        <f>IF(D39=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G39" t="s">
@@ -6813,7 +6842,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="str">
-        <f>IF(D40=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G40" t="s">
@@ -6855,7 +6884,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="str">
-        <f>IF(D41=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G41" t="s">
@@ -6897,7 +6926,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="str">
-        <f>IF(D42=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G42" t="s">
@@ -6939,7 +6968,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="str">
-        <f>IF(D43=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G43" t="s">
@@ -6981,7 +7010,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="str">
-        <f>IF(D44=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G44" t="s">
@@ -7023,7 +7052,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="str">
-        <f>IF(D45=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G45" t="s">
@@ -7065,7 +7094,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="str">
-        <f>IF(D46=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G46" t="s">
@@ -7107,7 +7136,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="str">
-        <f>IF(D47=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G47" t="s">
@@ -7149,7 +7178,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="str">
-        <f>IF(D48=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G48" t="s">
@@ -7191,7 +7220,7 @@
         <v>1</v>
       </c>
       <c r="F49" t="str">
-        <f>IF(D49=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G49" t="s">
@@ -7233,7 +7262,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="str">
-        <f>IF(D50=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G50" t="s">
@@ -7275,7 +7304,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="str">
-        <f>IF(D51=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G51" t="s">
@@ -7317,7 +7346,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="str">
-        <f>IF(D52=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G52" t="s">
@@ -7359,7 +7388,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="str">
-        <f>IF(D53=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G53" t="s">
@@ -7401,7 +7430,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="str">
-        <f>IF(D54=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G54" t="s">
@@ -7443,7 +7472,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="str">
-        <f>IF(D55=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G55" t="s">
@@ -7485,7 +7514,7 @@
         <v>1</v>
       </c>
       <c r="F56" t="str">
-        <f>IF(D56=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G56" t="s">
@@ -7527,7 +7556,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="str">
-        <f>IF(D57=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G57" t="s">
@@ -7569,7 +7598,7 @@
         <v>1</v>
       </c>
       <c r="F58" t="str">
-        <f>IF(D58=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G58" t="s">
@@ -7611,7 +7640,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="str">
-        <f>IF(D59=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G59" t="s">
@@ -7653,7 +7682,7 @@
         <v>1</v>
       </c>
       <c r="F60" t="str">
-        <f>IF(D60=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G60" t="s">
@@ -7695,7 +7724,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="str">
-        <f>IF(D61=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G61" t="s">
@@ -7737,7 +7766,7 @@
         <v>1</v>
       </c>
       <c r="F62" t="str">
-        <f>IF(D62=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G62" t="s">
@@ -7779,7 +7808,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="str">
-        <f>IF(D63=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G63" t="s">
@@ -7821,7 +7850,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="str">
-        <f>IF(D64=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G64" t="s">
@@ -7863,7 +7892,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="str">
-        <f>IF(D65=0,"false_diff","false_same")</f>
+        <f t="shared" si="0"/>
         <v>false_diff</v>
       </c>
       <c r="G65" t="s">
@@ -7905,7 +7934,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="str">
-        <f>IF(D66=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F66:F129" si="1">IF(D66=0,"false_diff","false_same")</f>
         <v>false_diff</v>
       </c>
       <c r="G66" t="s">
@@ -7947,7 +7976,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="str">
-        <f>IF(D67=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G67" t="s">
@@ -7989,7 +8018,7 @@
         <v>1</v>
       </c>
       <c r="F68" t="str">
-        <f>IF(D68=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G68" t="s">
@@ -8031,7 +8060,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="str">
-        <f>IF(D69=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G69" t="s">
@@ -8073,7 +8102,7 @@
         <v>1</v>
       </c>
       <c r="F70" t="str">
-        <f>IF(D70=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G70" t="s">
@@ -8115,7 +8144,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="str">
-        <f>IF(D71=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G71" t="s">
@@ -8157,7 +8186,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="str">
-        <f>IF(D72=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G72" t="s">
@@ -8199,7 +8228,7 @@
         <v>1</v>
       </c>
       <c r="F73" t="str">
-        <f>IF(D73=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G73" t="s">
@@ -8241,7 +8270,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="str">
-        <f>IF(D74=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G74" t="s">
@@ -8283,7 +8312,7 @@
         <v>1</v>
       </c>
       <c r="F75" t="str">
-        <f>IF(D75=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G75" t="s">
@@ -8325,7 +8354,7 @@
         <v>1</v>
       </c>
       <c r="F76" t="str">
-        <f>IF(D76=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G76" t="s">
@@ -8367,7 +8396,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="str">
-        <f>IF(D77=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G77" t="s">
@@ -8409,7 +8438,7 @@
         <v>1</v>
       </c>
       <c r="F78" t="str">
-        <f>IF(D78=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G78" t="s">
@@ -8451,7 +8480,7 @@
         <v>1</v>
       </c>
       <c r="F79" t="str">
-        <f>IF(D79=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G79" t="s">
@@ -8493,7 +8522,7 @@
         <v>1</v>
       </c>
       <c r="F80" t="str">
-        <f>IF(D80=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G80" t="s">
@@ -8535,7 +8564,7 @@
         <v>1</v>
       </c>
       <c r="F81" t="str">
-        <f>IF(D81=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G81" t="s">
@@ -8577,7 +8606,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="str">
-        <f>IF(D82=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G82" t="s">
@@ -8619,7 +8648,7 @@
         <v>1</v>
       </c>
       <c r="F83" t="str">
-        <f>IF(D83=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G83" t="s">
@@ -8661,7 +8690,7 @@
         <v>1</v>
       </c>
       <c r="F84" t="str">
-        <f>IF(D84=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G84" t="s">
@@ -8703,7 +8732,7 @@
         <v>1</v>
       </c>
       <c r="F85" t="str">
-        <f>IF(D85=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G85" t="s">
@@ -8745,7 +8774,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="str">
-        <f>IF(D86=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G86" t="s">
@@ -8787,7 +8816,7 @@
         <v>1</v>
       </c>
       <c r="F87" t="str">
-        <f>IF(D87=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G87" t="s">
@@ -8829,7 +8858,7 @@
         <v>1</v>
       </c>
       <c r="F88" t="str">
-        <f>IF(D88=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G88" t="s">
@@ -8871,7 +8900,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="str">
-        <f>IF(D89=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G89" t="s">
@@ -8913,7 +8942,7 @@
         <v>1</v>
       </c>
       <c r="F90" t="str">
-        <f>IF(D90=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G90" t="s">
@@ -8955,7 +8984,7 @@
         <v>1</v>
       </c>
       <c r="F91" t="str">
-        <f>IF(D91=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G91" t="s">
@@ -8997,7 +9026,7 @@
         <v>1</v>
       </c>
       <c r="F92" t="str">
-        <f>IF(D92=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G92" t="s">
@@ -9039,7 +9068,7 @@
         <v>1</v>
       </c>
       <c r="F93" t="str">
-        <f>IF(D93=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G93" t="s">
@@ -9081,7 +9110,7 @@
         <v>1</v>
       </c>
       <c r="F94" t="str">
-        <f>IF(D94=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G94" t="s">
@@ -9123,7 +9152,7 @@
         <v>1</v>
       </c>
       <c r="F95" t="str">
-        <f>IF(D95=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G95" t="s">
@@ -9165,7 +9194,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="str">
-        <f>IF(D96=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G96" t="s">
@@ -9207,7 +9236,7 @@
         <v>1</v>
       </c>
       <c r="F97" t="str">
-        <f>IF(D97=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G97" t="s">
@@ -9249,7 +9278,7 @@
         <v>1</v>
       </c>
       <c r="F98" t="str">
-        <f>IF(D98=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G98" t="s">
@@ -9291,7 +9320,7 @@
         <v>1</v>
       </c>
       <c r="F99" t="str">
-        <f>IF(D99=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G99" t="s">
@@ -9333,7 +9362,7 @@
         <v>1</v>
       </c>
       <c r="F100" t="str">
-        <f>IF(D100=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G100" t="s">
@@ -9375,7 +9404,7 @@
         <v>1</v>
       </c>
       <c r="F101" t="str">
-        <f>IF(D101=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G101" t="s">
@@ -9417,7 +9446,7 @@
         <v>1</v>
       </c>
       <c r="F102" t="str">
-        <f>IF(D102=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G102" t="s">
@@ -9459,7 +9488,7 @@
         <v>1</v>
       </c>
       <c r="F103" t="str">
-        <f>IF(D103=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G103" t="s">
@@ -9501,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="F104" t="str">
-        <f>IF(D104=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G104" t="s">
@@ -9543,7 +9572,7 @@
         <v>1</v>
       </c>
       <c r="F105" t="str">
-        <f>IF(D105=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G105" t="s">
@@ -9585,7 +9614,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="str">
-        <f>IF(D106=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G106" t="s">
@@ -9627,7 +9656,7 @@
         <v>1</v>
       </c>
       <c r="F107" t="str">
-        <f>IF(D107=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G107" t="s">
@@ -9669,7 +9698,7 @@
         <v>1</v>
       </c>
       <c r="F108" t="str">
-        <f>IF(D108=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G108" t="s">
@@ -9711,7 +9740,7 @@
         <v>1</v>
       </c>
       <c r="F109" t="str">
-        <f>IF(D109=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G109" t="s">
@@ -9753,7 +9782,7 @@
         <v>1</v>
       </c>
       <c r="F110" t="str">
-        <f>IF(D110=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G110" t="s">
@@ -9795,7 +9824,7 @@
         <v>1</v>
       </c>
       <c r="F111" t="str">
-        <f>IF(D111=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G111" t="s">
@@ -9837,7 +9866,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="str">
-        <f>IF(D112=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G112" t="s">
@@ -9879,7 +9908,7 @@
         <v>1</v>
       </c>
       <c r="F113" t="str">
-        <f>IF(D113=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G113" t="s">
@@ -9921,7 +9950,7 @@
         <v>1</v>
       </c>
       <c r="F114" t="str">
-        <f>IF(D114=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G114" t="s">
@@ -9963,7 +9992,7 @@
         <v>1</v>
       </c>
       <c r="F115" t="str">
-        <f>IF(D115=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G115" t="s">
@@ -10005,7 +10034,7 @@
         <v>1</v>
       </c>
       <c r="F116" t="str">
-        <f>IF(D116=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G116" t="s">
@@ -10047,7 +10076,7 @@
         <v>1</v>
       </c>
       <c r="F117" t="str">
-        <f>IF(D117=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G117" t="s">
@@ -10089,7 +10118,7 @@
         <v>1</v>
       </c>
       <c r="F118" t="str">
-        <f>IF(D118=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G118" t="s">
@@ -10131,7 +10160,7 @@
         <v>1</v>
       </c>
       <c r="F119" t="str">
-        <f>IF(D119=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G119" t="s">
@@ -10173,7 +10202,7 @@
         <v>1</v>
       </c>
       <c r="F120" t="str">
-        <f>IF(D120=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G120" t="s">
@@ -10215,7 +10244,7 @@
         <v>1</v>
       </c>
       <c r="F121" t="str">
-        <f>IF(D121=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G121" t="s">
@@ -10257,7 +10286,7 @@
         <v>1</v>
       </c>
       <c r="F122" t="str">
-        <f>IF(D122=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G122" t="s">
@@ -10299,7 +10328,7 @@
         <v>1</v>
       </c>
       <c r="F123" t="str">
-        <f>IF(D123=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G123" t="s">
@@ -10341,7 +10370,7 @@
         <v>1</v>
       </c>
       <c r="F124" t="str">
-        <f>IF(D124=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G124" t="s">
@@ -10383,7 +10412,7 @@
         <v>1</v>
       </c>
       <c r="F125" t="str">
-        <f>IF(D125=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G125" t="s">
@@ -10425,7 +10454,7 @@
         <v>1</v>
       </c>
       <c r="F126" t="str">
-        <f>IF(D126=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G126" t="s">
@@ -10467,7 +10496,7 @@
         <v>1</v>
       </c>
       <c r="F127" t="str">
-        <f>IF(D127=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G127" t="s">
@@ -10509,7 +10538,7 @@
         <v>1</v>
       </c>
       <c r="F128" t="str">
-        <f>IF(D128=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G128" t="s">
@@ -10551,7 +10580,7 @@
         <v>1</v>
       </c>
       <c r="F129" t="str">
-        <f>IF(D129=0,"false_diff","false_same")</f>
+        <f t="shared" si="1"/>
         <v>false_diff</v>
       </c>
       <c r="G129" t="s">
@@ -10593,7 +10622,7 @@
         <v>1</v>
       </c>
       <c r="F130" t="str">
-        <f>IF(D130=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F130:F193" si="2">IF(D130=0,"false_diff","false_same")</f>
         <v>false_diff</v>
       </c>
       <c r="G130" t="s">
@@ -10635,7 +10664,7 @@
         <v>1</v>
       </c>
       <c r="F131" t="str">
-        <f>IF(D131=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G131" t="s">
@@ -10677,7 +10706,7 @@
         <v>1</v>
       </c>
       <c r="F132" t="str">
-        <f>IF(D132=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G132" t="s">
@@ -10719,7 +10748,7 @@
         <v>1</v>
       </c>
       <c r="F133" t="str">
-        <f>IF(D133=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G133" t="s">
@@ -10761,7 +10790,7 @@
         <v>1</v>
       </c>
       <c r="F134" t="str">
-        <f>IF(D134=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G134" t="s">
@@ -10803,7 +10832,7 @@
         <v>1</v>
       </c>
       <c r="F135" t="str">
-        <f>IF(D135=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G135" t="s">
@@ -10845,7 +10874,7 @@
         <v>1</v>
       </c>
       <c r="F136" t="str">
-        <f>IF(D136=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G136" t="s">
@@ -10887,7 +10916,7 @@
         <v>1</v>
       </c>
       <c r="F137" t="str">
-        <f>IF(D137=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G137" t="s">
@@ -10929,7 +10958,7 @@
         <v>1</v>
       </c>
       <c r="F138" t="str">
-        <f>IF(D138=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G138" t="s">
@@ -10971,7 +11000,7 @@
         <v>1</v>
       </c>
       <c r="F139" t="str">
-        <f>IF(D139=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G139" t="s">
@@ -11013,7 +11042,7 @@
         <v>1</v>
       </c>
       <c r="F140" t="str">
-        <f>IF(D140=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G140" t="s">
@@ -11055,7 +11084,7 @@
         <v>1</v>
       </c>
       <c r="F141" t="str">
-        <f>IF(D141=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G141" t="s">
@@ -11097,7 +11126,7 @@
         <v>1</v>
       </c>
       <c r="F142" t="str">
-        <f>IF(D142=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G142" t="s">
@@ -11139,7 +11168,7 @@
         <v>1</v>
       </c>
       <c r="F143" t="str">
-        <f>IF(D143=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G143" t="s">
@@ -11181,7 +11210,7 @@
         <v>1</v>
       </c>
       <c r="F144" t="str">
-        <f>IF(D144=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G144" t="s">
@@ -11223,7 +11252,7 @@
         <v>1</v>
       </c>
       <c r="F145" t="str">
-        <f>IF(D145=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G145" t="s">
@@ -11265,7 +11294,7 @@
         <v>1</v>
       </c>
       <c r="F146" t="str">
-        <f>IF(D146=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G146" t="s">
@@ -11307,7 +11336,7 @@
         <v>1</v>
       </c>
       <c r="F147" t="str">
-        <f>IF(D147=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G147" t="s">
@@ -11349,7 +11378,7 @@
         <v>1</v>
       </c>
       <c r="F148" t="str">
-        <f>IF(D148=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G148" t="s">
@@ -11391,7 +11420,7 @@
         <v>1</v>
       </c>
       <c r="F149" t="str">
-        <f>IF(D149=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G149" t="s">
@@ -11433,7 +11462,7 @@
         <v>1</v>
       </c>
       <c r="F150" t="str">
-        <f>IF(D150=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G150" t="s">
@@ -11475,7 +11504,7 @@
         <v>1</v>
       </c>
       <c r="F151" t="str">
-        <f>IF(D151=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G151" t="s">
@@ -11517,7 +11546,7 @@
         <v>1</v>
       </c>
       <c r="F152" t="str">
-        <f>IF(D152=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G152" t="s">
@@ -11559,7 +11588,7 @@
         <v>1</v>
       </c>
       <c r="F153" t="str">
-        <f>IF(D153=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G153" t="s">
@@ -11601,7 +11630,7 @@
         <v>1</v>
       </c>
       <c r="F154" t="str">
-        <f>IF(D154=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G154" t="s">
@@ -11643,7 +11672,7 @@
         <v>1</v>
       </c>
       <c r="F155" t="str">
-        <f>IF(D155=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G155" t="s">
@@ -11685,7 +11714,7 @@
         <v>1</v>
       </c>
       <c r="F156" t="str">
-        <f>IF(D156=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G156" t="s">
@@ -11727,7 +11756,7 @@
         <v>1</v>
       </c>
       <c r="F157" t="str">
-        <f>IF(D157=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G157" t="s">
@@ -11769,7 +11798,7 @@
         <v>1</v>
       </c>
       <c r="F158" t="str">
-        <f>IF(D158=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G158" t="s">
@@ -11811,7 +11840,7 @@
         <v>1</v>
       </c>
       <c r="F159" t="str">
-        <f>IF(D159=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G159" t="s">
@@ -11853,7 +11882,7 @@
         <v>1</v>
       </c>
       <c r="F160" t="str">
-        <f>IF(D160=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G160" t="s">
@@ -11895,7 +11924,7 @@
         <v>1</v>
       </c>
       <c r="F161" t="str">
-        <f>IF(D161=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G161" t="s">
@@ -11937,7 +11966,7 @@
         <v>1</v>
       </c>
       <c r="F162" t="str">
-        <f>IF(D162=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G162" t="s">
@@ -11979,7 +12008,7 @@
         <v>1</v>
       </c>
       <c r="F163" t="str">
-        <f>IF(D163=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G163" t="s">
@@ -12021,7 +12050,7 @@
         <v>1</v>
       </c>
       <c r="F164" t="str">
-        <f>IF(D164=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G164" t="s">
@@ -12072,7 +12101,7 @@
         <v>1</v>
       </c>
       <c r="F165" t="str">
-        <f>IF(D165=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G165" t="s">
@@ -12124,7 +12153,7 @@
         <v>1</v>
       </c>
       <c r="F166" t="str">
-        <f>IF(D166=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G166" t="s">
@@ -12176,7 +12205,7 @@
         <v>1</v>
       </c>
       <c r="F167" t="str">
-        <f>IF(D167=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G167" t="s">
@@ -12228,7 +12257,7 @@
         <v>1</v>
       </c>
       <c r="F168" t="str">
-        <f>IF(D168=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G168" t="s">
@@ -12280,7 +12309,7 @@
         <v>1</v>
       </c>
       <c r="F169" t="str">
-        <f>IF(D169=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G169" t="s">
@@ -12332,7 +12361,7 @@
         <v>1</v>
       </c>
       <c r="F170" t="str">
-        <f>IF(D170=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G170" t="s">
@@ -12384,7 +12413,7 @@
         <v>1</v>
       </c>
       <c r="F171" t="str">
-        <f>IF(D171=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G171" t="s">
@@ -12436,7 +12465,7 @@
         <v>1</v>
       </c>
       <c r="F172" t="str">
-        <f>IF(D172=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G172" t="s">
@@ -12488,7 +12517,7 @@
         <v>1</v>
       </c>
       <c r="F173" t="str">
-        <f>IF(D173=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G173" t="s">
@@ -12540,7 +12569,7 @@
         <v>1</v>
       </c>
       <c r="F174" t="str">
-        <f>IF(D174=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G174" t="s">
@@ -12592,7 +12621,7 @@
         <v>1</v>
       </c>
       <c r="F175" t="str">
-        <f>IF(D175=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G175" t="s">
@@ -12644,7 +12673,7 @@
         <v>1</v>
       </c>
       <c r="F176" t="str">
-        <f>IF(D176=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G176" t="s">
@@ -12696,7 +12725,7 @@
         <v>1</v>
       </c>
       <c r="F177" t="str">
-        <f>IF(D177=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G177" t="s">
@@ -12748,7 +12777,7 @@
         <v>1</v>
       </c>
       <c r="F178" t="str">
-        <f>IF(D178=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G178" t="s">
@@ -12800,7 +12829,7 @@
         <v>1</v>
       </c>
       <c r="F179" t="str">
-        <f>IF(D179=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G179" t="s">
@@ -12852,7 +12881,7 @@
         <v>1</v>
       </c>
       <c r="F180" t="str">
-        <f>IF(D180=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G180" t="s">
@@ -12904,7 +12933,7 @@
         <v>1</v>
       </c>
       <c r="F181" t="str">
-        <f>IF(D181=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G181" t="s">
@@ -12956,7 +12985,7 @@
         <v>1</v>
       </c>
       <c r="F182" t="str">
-        <f>IF(D182=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G182" t="s">
@@ -13008,7 +13037,7 @@
         <v>1</v>
       </c>
       <c r="F183" t="str">
-        <f>IF(D183=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G183" t="s">
@@ -13060,7 +13089,7 @@
         <v>1</v>
       </c>
       <c r="F184" t="str">
-        <f>IF(D184=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G184" t="s">
@@ -13112,7 +13141,7 @@
         <v>1</v>
       </c>
       <c r="F185" t="str">
-        <f>IF(D185=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G185" t="s">
@@ -13164,7 +13193,7 @@
         <v>1</v>
       </c>
       <c r="F186" t="str">
-        <f>IF(D186=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G186" t="s">
@@ -13216,7 +13245,7 @@
         <v>1</v>
       </c>
       <c r="F187" t="str">
-        <f>IF(D187=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G187" t="s">
@@ -13268,7 +13297,7 @@
         <v>1</v>
       </c>
       <c r="F188" t="str">
-        <f>IF(D188=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G188" t="s">
@@ -13320,7 +13349,7 @@
         <v>1</v>
       </c>
       <c r="F189" t="str">
-        <f>IF(D189=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G189" t="s">
@@ -13372,7 +13401,7 @@
         <v>1</v>
       </c>
       <c r="F190" t="str">
-        <f>IF(D190=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G190" t="s">
@@ -13424,7 +13453,7 @@
         <v>1</v>
       </c>
       <c r="F191" t="str">
-        <f>IF(D191=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G191" t="s">
@@ -13466,7 +13495,7 @@
         <v>1</v>
       </c>
       <c r="F192" t="str">
-        <f>IF(D192=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G192" t="s">
@@ -13508,7 +13537,7 @@
         <v>1</v>
       </c>
       <c r="F193" t="str">
-        <f>IF(D193=0,"false_diff","false_same")</f>
+        <f t="shared" si="2"/>
         <v>false_diff</v>
       </c>
       <c r="G193" t="s">
@@ -13553,7 +13582,7 @@
         <v>1</v>
       </c>
       <c r="F194" t="str">
-        <f>IF(D194=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F194:F257" si="3">IF(D194=0,"false_diff","false_same")</f>
         <v>false_diff</v>
       </c>
       <c r="G194" t="s">
@@ -13609,7 +13638,7 @@
         <v>1</v>
       </c>
       <c r="F195" t="str">
-        <f>IF(D195=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G195" t="s">
@@ -13644,7 +13673,7 @@
         <v>0</v>
       </c>
       <c r="R195">
-        <f t="shared" ref="R195:R196" si="0">SUM(P195:Q195)</f>
+        <f t="shared" ref="R195:R196" si="4">SUM(P195:Q195)</f>
         <v>23</v>
       </c>
     </row>
@@ -13665,7 +13694,7 @@
         <v>1</v>
       </c>
       <c r="F196" t="str">
-        <f>IF(D196=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G196" t="s">
@@ -13700,7 +13729,7 @@
         <v>24</v>
       </c>
       <c r="R196">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="S196">
@@ -13725,7 +13754,7 @@
         <v>1</v>
       </c>
       <c r="F197" t="str">
-        <f>IF(D197=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G197" t="s">
@@ -13767,7 +13796,7 @@
         <v>1</v>
       </c>
       <c r="F198" t="str">
-        <f>IF(D198=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G198" t="s">
@@ -13824,7 +13853,7 @@
         <v>1</v>
       </c>
       <c r="F199" t="str">
-        <f>IF(D199=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G199" t="s">
@@ -13870,7 +13899,7 @@
         <v>1</v>
       </c>
       <c r="F200" t="str">
-        <f>IF(D200=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G200" t="s">
@@ -13916,7 +13945,7 @@
         <v>1</v>
       </c>
       <c r="F201" t="str">
-        <f>IF(D201=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G201" t="s">
@@ -13958,7 +13987,7 @@
         <v>1</v>
       </c>
       <c r="F202" t="str">
-        <f>IF(D202=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G202" t="s">
@@ -14000,7 +14029,7 @@
         <v>1</v>
       </c>
       <c r="F203" t="str">
-        <f>IF(D203=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G203" t="s">
@@ -14042,7 +14071,7 @@
         <v>1</v>
       </c>
       <c r="F204" t="str">
-        <f>IF(D204=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G204" t="s">
@@ -14084,7 +14113,7 @@
         <v>1</v>
       </c>
       <c r="F205" t="str">
-        <f>IF(D205=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G205" t="s">
@@ -14126,7 +14155,7 @@
         <v>1</v>
       </c>
       <c r="F206" t="str">
-        <f>IF(D206=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G206" t="s">
@@ -14168,7 +14197,7 @@
         <v>1</v>
       </c>
       <c r="F207" t="str">
-        <f>IF(D207=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G207" t="s">
@@ -14210,7 +14239,7 @@
         <v>1</v>
       </c>
       <c r="F208" t="str">
-        <f>IF(D208=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G208" t="s">
@@ -14252,7 +14281,7 @@
         <v>1</v>
       </c>
       <c r="F209" t="str">
-        <f>IF(D209=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G209" t="s">
@@ -14294,7 +14323,7 @@
         <v>1</v>
       </c>
       <c r="F210" t="str">
-        <f>IF(D210=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G210" t="s">
@@ -14336,7 +14365,7 @@
         <v>1</v>
       </c>
       <c r="F211" t="str">
-        <f>IF(D211=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G211" t="s">
@@ -14378,7 +14407,7 @@
         <v>1</v>
       </c>
       <c r="F212" t="str">
-        <f>IF(D212=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G212" t="s">
@@ -14420,7 +14449,7 @@
         <v>1</v>
       </c>
       <c r="F213" t="str">
-        <f>IF(D213=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G213" t="s">
@@ -14462,7 +14491,7 @@
         <v>1</v>
       </c>
       <c r="F214" t="str">
-        <f>IF(D214=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G214" t="s">
@@ -14504,7 +14533,7 @@
         <v>1</v>
       </c>
       <c r="F215" t="str">
-        <f>IF(D215=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G215" t="s">
@@ -14546,7 +14575,7 @@
         <v>1</v>
       </c>
       <c r="F216" t="str">
-        <f>IF(D216=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G216" t="s">
@@ -14588,7 +14617,7 @@
         <v>1</v>
       </c>
       <c r="F217" t="str">
-        <f>IF(D217=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G217" t="s">
@@ -14630,7 +14659,7 @@
         <v>1</v>
       </c>
       <c r="F218" t="str">
-        <f>IF(D218=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G218" t="s">
@@ -14672,7 +14701,7 @@
         <v>1</v>
       </c>
       <c r="F219" t="str">
-        <f>IF(D219=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G219" t="s">
@@ -14714,7 +14743,7 @@
         <v>1</v>
       </c>
       <c r="F220" t="str">
-        <f>IF(D220=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G220" t="s">
@@ -14756,7 +14785,7 @@
         <v>1</v>
       </c>
       <c r="F221" t="str">
-        <f>IF(D221=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G221" t="s">
@@ -14798,7 +14827,7 @@
         <v>1</v>
       </c>
       <c r="F222" t="str">
-        <f>IF(D222=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G222" t="s">
@@ -14840,7 +14869,7 @@
         <v>1</v>
       </c>
       <c r="F223" t="str">
-        <f>IF(D223=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G223" t="s">
@@ -14882,7 +14911,7 @@
         <v>1</v>
       </c>
       <c r="F224" t="str">
-        <f>IF(D224=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G224" t="s">
@@ -14924,7 +14953,7 @@
         <v>1</v>
       </c>
       <c r="F225" t="str">
-        <f>IF(D225=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G225" t="s">
@@ -14966,7 +14995,7 @@
         <v>1</v>
       </c>
       <c r="F226" t="str">
-        <f>IF(D226=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G226" t="s">
@@ -15008,7 +15037,7 @@
         <v>1</v>
       </c>
       <c r="F227" t="str">
-        <f>IF(D227=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G227" t="s">
@@ -15050,7 +15079,7 @@
         <v>1</v>
       </c>
       <c r="F228" t="str">
-        <f>IF(D228=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G228" t="s">
@@ -15092,7 +15121,7 @@
         <v>1</v>
       </c>
       <c r="F229" t="str">
-        <f>IF(D229=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G229" t="s">
@@ -15134,7 +15163,7 @@
         <v>1</v>
       </c>
       <c r="F230" t="str">
-        <f>IF(D230=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G230" t="s">
@@ -15176,7 +15205,7 @@
         <v>1</v>
       </c>
       <c r="F231" t="str">
-        <f>IF(D231=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G231" t="s">
@@ -15218,7 +15247,7 @@
         <v>1</v>
       </c>
       <c r="F232" t="str">
-        <f>IF(D232=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G232" t="s">
@@ -15260,7 +15289,7 @@
         <v>1</v>
       </c>
       <c r="F233" t="str">
-        <f>IF(D233=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G233" t="s">
@@ -15302,7 +15331,7 @@
         <v>1</v>
       </c>
       <c r="F234" t="str">
-        <f>IF(D234=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G234" t="s">
@@ -15344,7 +15373,7 @@
         <v>1</v>
       </c>
       <c r="F235" t="str">
-        <f>IF(D235=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G235" t="s">
@@ -15386,7 +15415,7 @@
         <v>1</v>
       </c>
       <c r="F236" t="str">
-        <f>IF(D236=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G236" t="s">
@@ -15428,7 +15457,7 @@
         <v>1</v>
       </c>
       <c r="F237" t="str">
-        <f>IF(D237=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G237" t="s">
@@ -15470,7 +15499,7 @@
         <v>1</v>
       </c>
       <c r="F238" t="str">
-        <f>IF(D238=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G238" t="s">
@@ -15512,7 +15541,7 @@
         <v>1</v>
       </c>
       <c r="F239" t="str">
-        <f>IF(D239=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G239" t="s">
@@ -15554,7 +15583,7 @@
         <v>1</v>
       </c>
       <c r="F240" t="str">
-        <f>IF(D240=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G240" t="s">
@@ -15596,7 +15625,7 @@
         <v>1</v>
       </c>
       <c r="F241" t="str">
-        <f>IF(D241=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G241" t="s">
@@ -15638,7 +15667,7 @@
         <v>1</v>
       </c>
       <c r="F242" t="str">
-        <f>IF(D242=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G242" t="s">
@@ -15680,7 +15709,7 @@
         <v>1</v>
       </c>
       <c r="F243" t="str">
-        <f>IF(D243=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G243" t="s">
@@ -15722,7 +15751,7 @@
         <v>1</v>
       </c>
       <c r="F244" t="str">
-        <f>IF(D244=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G244" t="s">
@@ -15764,7 +15793,7 @@
         <v>1</v>
       </c>
       <c r="F245" t="str">
-        <f>IF(D245=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G245" t="s">
@@ -15806,7 +15835,7 @@
         <v>1</v>
       </c>
       <c r="F246" t="str">
-        <f>IF(D246=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G246" t="s">
@@ -15848,7 +15877,7 @@
         <v>1</v>
       </c>
       <c r="F247" t="str">
-        <f>IF(D247=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G247" t="s">
@@ -15890,7 +15919,7 @@
         <v>1</v>
       </c>
       <c r="F248" t="str">
-        <f>IF(D248=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G248" t="s">
@@ -15932,7 +15961,7 @@
         <v>1</v>
       </c>
       <c r="F249" t="str">
-        <f>IF(D249=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G249" t="s">
@@ -15974,7 +16003,7 @@
         <v>1</v>
       </c>
       <c r="F250" t="str">
-        <f>IF(D250=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G250" t="s">
@@ -16016,7 +16045,7 @@
         <v>1</v>
       </c>
       <c r="F251" t="str">
-        <f>IF(D251=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G251" t="s">
@@ -16058,7 +16087,7 @@
         <v>1</v>
       </c>
       <c r="F252" t="str">
-        <f>IF(D252=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G252" t="s">
@@ -16100,7 +16129,7 @@
         <v>1</v>
       </c>
       <c r="F253" t="str">
-        <f>IF(D253=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G253" t="s">
@@ -16142,7 +16171,7 @@
         <v>1</v>
       </c>
       <c r="F254" t="str">
-        <f>IF(D254=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G254" t="s">
@@ -16184,7 +16213,7 @@
         <v>1</v>
       </c>
       <c r="F255" t="str">
-        <f>IF(D255=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G255" t="s">
@@ -16226,7 +16255,7 @@
         <v>1</v>
       </c>
       <c r="F256" t="str">
-        <f>IF(D256=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G256" t="s">
@@ -16268,7 +16297,7 @@
         <v>1</v>
       </c>
       <c r="F257" t="str">
-        <f>IF(D257=0,"false_diff","false_same")</f>
+        <f t="shared" si="3"/>
         <v>false_diff</v>
       </c>
       <c r="G257" t="s">
@@ -16310,7 +16339,7 @@
         <v>1</v>
       </c>
       <c r="F258" t="str">
-        <f>IF(D258=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F258:F321" si="5">IF(D258=0,"false_diff","false_same")</f>
         <v>false_diff</v>
       </c>
       <c r="G258" t="s">
@@ -16352,7 +16381,7 @@
         <v>1</v>
       </c>
       <c r="F259" t="str">
-        <f>IF(D259=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G259" t="s">
@@ -16394,7 +16423,7 @@
         <v>1</v>
       </c>
       <c r="F260" t="str">
-        <f>IF(D260=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G260" t="s">
@@ -16436,7 +16465,7 @@
         <v>1</v>
       </c>
       <c r="F261" t="str">
-        <f>IF(D261=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G261" t="s">
@@ -16478,7 +16507,7 @@
         <v>1</v>
       </c>
       <c r="F262" t="str">
-        <f>IF(D262=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G262" t="s">
@@ -16520,7 +16549,7 @@
         <v>1</v>
       </c>
       <c r="F263" t="str">
-        <f>IF(D263=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G263" t="s">
@@ -16562,7 +16591,7 @@
         <v>1</v>
       </c>
       <c r="F264" t="str">
-        <f>IF(D264=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G264" t="s">
@@ -16604,7 +16633,7 @@
         <v>1</v>
       </c>
       <c r="F265" t="str">
-        <f>IF(D265=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G265" t="s">
@@ -16646,7 +16675,7 @@
         <v>1</v>
       </c>
       <c r="F266" t="str">
-        <f>IF(D266=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G266" t="s">
@@ -16688,7 +16717,7 @@
         <v>1</v>
       </c>
       <c r="F267" t="str">
-        <f>IF(D267=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G267" t="s">
@@ -16730,7 +16759,7 @@
         <v>1</v>
       </c>
       <c r="F268" t="str">
-        <f>IF(D268=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G268" t="s">
@@ -16772,7 +16801,7 @@
         <v>1</v>
       </c>
       <c r="F269" t="str">
-        <f>IF(D269=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G269" t="s">
@@ -16814,7 +16843,7 @@
         <v>1</v>
       </c>
       <c r="F270" t="str">
-        <f>IF(D270=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G270" t="s">
@@ -16856,7 +16885,7 @@
         <v>1</v>
       </c>
       <c r="F271" t="str">
-        <f>IF(D271=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G271" t="s">
@@ -16898,7 +16927,7 @@
         <v>1</v>
       </c>
       <c r="F272" t="str">
-        <f>IF(D272=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G272" t="s">
@@ -16940,7 +16969,7 @@
         <v>1</v>
       </c>
       <c r="F273" t="str">
-        <f>IF(D273=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G273" t="s">
@@ -16982,7 +17011,7 @@
         <v>1</v>
       </c>
       <c r="F274" t="str">
-        <f>IF(D274=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G274" t="s">
@@ -17024,7 +17053,7 @@
         <v>1</v>
       </c>
       <c r="F275" t="str">
-        <f>IF(D275=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G275" t="s">
@@ -17066,7 +17095,7 @@
         <v>1</v>
       </c>
       <c r="F276" t="str">
-        <f>IF(D276=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G276" t="s">
@@ -17108,7 +17137,7 @@
         <v>1</v>
       </c>
       <c r="F277" t="str">
-        <f>IF(D277=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G277" t="s">
@@ -17150,7 +17179,7 @@
         <v>1</v>
       </c>
       <c r="F278" t="str">
-        <f>IF(D278=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G278" t="s">
@@ -17192,7 +17221,7 @@
         <v>1</v>
       </c>
       <c r="F279" t="str">
-        <f>IF(D279=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G279" t="s">
@@ -17234,7 +17263,7 @@
         <v>1</v>
       </c>
       <c r="F280" t="str">
-        <f>IF(D280=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G280" t="s">
@@ -17276,7 +17305,7 @@
         <v>1</v>
       </c>
       <c r="F281" t="str">
-        <f>IF(D281=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G281" t="s">
@@ -17318,7 +17347,7 @@
         <v>1</v>
       </c>
       <c r="F282" t="str">
-        <f>IF(D282=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G282" t="s">
@@ -17360,7 +17389,7 @@
         <v>1</v>
       </c>
       <c r="F283" t="str">
-        <f>IF(D283=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G283" t="s">
@@ -17402,7 +17431,7 @@
         <v>1</v>
       </c>
       <c r="F284" t="str">
-        <f>IF(D284=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G284" t="s">
@@ -17444,7 +17473,7 @@
         <v>1</v>
       </c>
       <c r="F285" t="str">
-        <f>IF(D285=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G285" t="s">
@@ -17486,7 +17515,7 @@
         <v>1</v>
       </c>
       <c r="F286" t="str">
-        <f>IF(D286=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G286" t="s">
@@ -17528,7 +17557,7 @@
         <v>1</v>
       </c>
       <c r="F287" t="str">
-        <f>IF(D287=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G287" t="s">
@@ -17570,7 +17599,7 @@
         <v>1</v>
       </c>
       <c r="F288" t="str">
-        <f>IF(D288=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G288" t="s">
@@ -17612,7 +17641,7 @@
         <v>1</v>
       </c>
       <c r="F289" t="str">
-        <f>IF(D289=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G289" t="s">
@@ -17654,7 +17683,7 @@
         <v>1</v>
       </c>
       <c r="F290" t="str">
-        <f>IF(D290=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G290" t="s">
@@ -17696,7 +17725,7 @@
         <v>1</v>
       </c>
       <c r="F291" t="str">
-        <f>IF(D291=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G291" t="s">
@@ -17738,7 +17767,7 @@
         <v>1</v>
       </c>
       <c r="F292" t="str">
-        <f>IF(D292=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G292" t="s">
@@ -17780,7 +17809,7 @@
         <v>1</v>
       </c>
       <c r="F293" t="str">
-        <f>IF(D293=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G293" t="s">
@@ -17822,7 +17851,7 @@
         <v>1</v>
       </c>
       <c r="F294" t="str">
-        <f>IF(D294=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G294" t="s">
@@ -17864,7 +17893,7 @@
         <v>1</v>
       </c>
       <c r="F295" t="str">
-        <f>IF(D295=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G295" t="s">
@@ -17906,7 +17935,7 @@
         <v>1</v>
       </c>
       <c r="F296" t="str">
-        <f>IF(D296=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G296" t="s">
@@ -17948,7 +17977,7 @@
         <v>1</v>
       </c>
       <c r="F297" t="str">
-        <f>IF(D297=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G297" t="s">
@@ -17990,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="F298" t="str">
-        <f>IF(D298=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G298" t="s">
@@ -18032,7 +18061,7 @@
         <v>1</v>
       </c>
       <c r="F299" t="str">
-        <f>IF(D299=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G299" t="s">
@@ -18074,7 +18103,7 @@
         <v>1</v>
       </c>
       <c r="F300" t="str">
-        <f>IF(D300=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G300" t="s">
@@ -18116,7 +18145,7 @@
         <v>1</v>
       </c>
       <c r="F301" t="str">
-        <f>IF(D301=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G301" t="s">
@@ -18158,7 +18187,7 @@
         <v>1</v>
       </c>
       <c r="F302" t="str">
-        <f>IF(D302=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G302" t="s">
@@ -18200,7 +18229,7 @@
         <v>1</v>
       </c>
       <c r="F303" t="str">
-        <f>IF(D303=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G303" t="s">
@@ -18242,7 +18271,7 @@
         <v>1</v>
       </c>
       <c r="F304" t="str">
-        <f>IF(D304=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G304" t="s">
@@ -18284,7 +18313,7 @@
         <v>1</v>
       </c>
       <c r="F305" t="str">
-        <f>IF(D305=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G305" t="s">
@@ -18326,7 +18355,7 @@
         <v>1</v>
       </c>
       <c r="F306" t="str">
-        <f>IF(D306=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G306" t="s">
@@ -18368,7 +18397,7 @@
         <v>1</v>
       </c>
       <c r="F307" t="str">
-        <f>IF(D307=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G307" t="s">
@@ -18410,7 +18439,7 @@
         <v>1</v>
       </c>
       <c r="F308" t="str">
-        <f>IF(D308=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G308" t="s">
@@ -18452,7 +18481,7 @@
         <v>1</v>
       </c>
       <c r="F309" t="str">
-        <f>IF(D309=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G309" t="s">
@@ -18494,7 +18523,7 @@
         <v>1</v>
       </c>
       <c r="F310" t="str">
-        <f>IF(D310=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G310" t="s">
@@ -18536,7 +18565,7 @@
         <v>1</v>
       </c>
       <c r="F311" t="str">
-        <f>IF(D311=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G311" t="s">
@@ -18578,7 +18607,7 @@
         <v>1</v>
       </c>
       <c r="F312" t="str">
-        <f>IF(D312=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G312" t="s">
@@ -18620,7 +18649,7 @@
         <v>1</v>
       </c>
       <c r="F313" t="str">
-        <f>IF(D313=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G313" t="s">
@@ -18662,7 +18691,7 @@
         <v>1</v>
       </c>
       <c r="F314" t="str">
-        <f>IF(D314=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G314" t="s">
@@ -18704,7 +18733,7 @@
         <v>1</v>
       </c>
       <c r="F315" t="str">
-        <f>IF(D315=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G315" t="s">
@@ -18746,7 +18775,7 @@
         <v>1</v>
       </c>
       <c r="F316" t="str">
-        <f>IF(D316=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G316" t="s">
@@ -18788,7 +18817,7 @@
         <v>1</v>
       </c>
       <c r="F317" t="str">
-        <f>IF(D317=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G317" t="s">
@@ -18830,7 +18859,7 @@
         <v>1</v>
       </c>
       <c r="F318" t="str">
-        <f>IF(D318=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_diff</v>
       </c>
       <c r="G318" t="s">
@@ -18872,7 +18901,7 @@
         <v>0</v>
       </c>
       <c r="F319" t="str">
-        <f>IF(D319=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_same</v>
       </c>
       <c r="G319" t="s">
@@ -18914,7 +18943,7 @@
         <v>0</v>
       </c>
       <c r="F320" t="str">
-        <f>IF(D320=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_same</v>
       </c>
       <c r="G320" t="s">
@@ -18956,7 +18985,7 @@
         <v>0</v>
       </c>
       <c r="F321" t="str">
-        <f>IF(D321=0,"false_diff","false_same")</f>
+        <f t="shared" si="5"/>
         <v>false_same</v>
       </c>
       <c r="G321" t="s">
@@ -18998,7 +19027,7 @@
         <v>0</v>
       </c>
       <c r="F322" t="str">
-        <f>IF(D322=0,"false_diff","false_same")</f>
+        <f t="shared" ref="F322:F342" si="6">IF(D322=0,"false_diff","false_same")</f>
         <v>false_same</v>
       </c>
       <c r="G322" t="s">
@@ -19040,7 +19069,7 @@
         <v>0</v>
       </c>
       <c r="F323" t="str">
-        <f>IF(D323=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G323" t="s">
@@ -19082,7 +19111,7 @@
         <v>0</v>
       </c>
       <c r="F324" t="str">
-        <f>IF(D324=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G324" t="s">
@@ -19124,7 +19153,7 @@
         <v>0</v>
       </c>
       <c r="F325" t="str">
-        <f>IF(D325=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G325" t="s">
@@ -19166,7 +19195,7 @@
         <v>0</v>
       </c>
       <c r="F326" t="str">
-        <f>IF(D326=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G326" t="s">
@@ -19208,7 +19237,7 @@
         <v>0</v>
       </c>
       <c r="F327" t="str">
-        <f>IF(D327=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G327" t="s">
@@ -19250,7 +19279,7 @@
         <v>0</v>
       </c>
       <c r="F328" t="str">
-        <f>IF(D328=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G328" t="s">
@@ -19292,7 +19321,7 @@
         <v>0</v>
       </c>
       <c r="F329" t="str">
-        <f>IF(D329=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G329" t="s">
@@ -19334,7 +19363,7 @@
         <v>0</v>
       </c>
       <c r="F330" t="str">
-        <f>IF(D330=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G330" t="s">
@@ -19376,7 +19405,7 @@
         <v>0</v>
       </c>
       <c r="F331" t="str">
-        <f>IF(D331=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G331" t="s">
@@ -19418,7 +19447,7 @@
         <v>0</v>
       </c>
       <c r="F332" t="str">
-        <f>IF(D332=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G332" t="s">
@@ -19460,7 +19489,7 @@
         <v>0</v>
       </c>
       <c r="F333" t="str">
-        <f>IF(D333=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G333" t="s">
@@ -19502,7 +19531,7 @@
         <v>0</v>
       </c>
       <c r="F334" t="str">
-        <f>IF(D334=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G334" t="s">
@@ -19544,7 +19573,7 @@
         <v>0</v>
       </c>
       <c r="F335" t="str">
-        <f>IF(D335=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G335" t="s">
@@ -19586,7 +19615,7 @@
         <v>0</v>
       </c>
       <c r="F336" t="str">
-        <f>IF(D336=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G336" t="s">
@@ -19628,7 +19657,7 @@
         <v>0</v>
       </c>
       <c r="F337" t="str">
-        <f>IF(D337=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G337" t="s">
@@ -19670,7 +19699,7 @@
         <v>0</v>
       </c>
       <c r="F338" t="str">
-        <f>IF(D338=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G338" t="s">
@@ -19712,7 +19741,7 @@
         <v>0</v>
       </c>
       <c r="F339" t="str">
-        <f>IF(D339=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G339" t="s">
@@ -19754,7 +19783,7 @@
         <v>0</v>
       </c>
       <c r="F340" t="str">
-        <f>IF(D340=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G340" t="s">
@@ -19796,7 +19825,7 @@
         <v>0</v>
       </c>
       <c r="F341" t="str">
-        <f>IF(D341=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G341" t="s">
@@ -19838,7 +19867,7 @@
         <v>0</v>
       </c>
       <c r="F342" t="str">
-        <f>IF(D342=0,"false_diff","false_same")</f>
+        <f t="shared" si="6"/>
         <v>false_same</v>
       </c>
       <c r="G342" t="s">

</xml_diff>